<commit_message>
Placed jacks and pot references
</commit_message>
<xml_diff>
--- a/Preliminary BoM.xlsx
+++ b/Preliminary BoM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Engineering\GitHub\DMH-VCEG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC2483A-8D82-4CBC-9588-AC6B880A8F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE51779-2FBA-456F-B734-D30CC8AFAF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{9025ED8D-87B0-4B6C-A3C2-D58E978FDF41}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="133">
   <si>
     <t>Reference</t>
   </si>
@@ -414,6 +414,15 @@
   </si>
   <si>
     <t>Qty buy</t>
+  </si>
+  <si>
+    <t>500k</t>
+  </si>
+  <si>
+    <t>390k</t>
+  </si>
+  <si>
+    <t>na</t>
   </si>
 </sst>
 </file>
@@ -556,7 +565,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -736,6 +745,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -897,9 +912,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -945,7 +962,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="19">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1008,6 +1025,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1033,6 +1070,46 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2223,11 +2300,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F8EA1B3-DE99-4B5B-B92A-5EF6DEBF9FE4}">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
+      <selection pane="bottomLeft" activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2276,10 +2353,13 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G2">
         <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2296,10 +2376,13 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G3">
         <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2316,10 +2399,13 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G4">
         <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2336,10 +2422,13 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G5">
         <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2361,6 +2450,9 @@
       <c r="G6">
         <v>2</v>
       </c>
+      <c r="H6" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2376,10 +2468,13 @@
         <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G7">
         <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2396,10 +2491,13 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G8">
         <v>0</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2419,7 +2517,10 @@
         <v>117</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2436,10 +2537,13 @@
         <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G10">
         <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2461,6 +2565,9 @@
       <c r="G11">
         <v>1</v>
       </c>
+      <c r="H11" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -2481,6 +2588,9 @@
       <c r="G12">
         <v>4</v>
       </c>
+      <c r="H12" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -2501,6 +2611,9 @@
       <c r="G13">
         <v>10</v>
       </c>
+      <c r="H13" s="2" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -2521,6 +2634,9 @@
       <c r="G14">
         <v>0</v>
       </c>
+      <c r="H14" s="2" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -2541,6 +2657,9 @@
       <c r="G15">
         <v>0</v>
       </c>
+      <c r="H15" s="2" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -2561,8 +2680,11 @@
       <c r="G16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -2581,8 +2703,11 @@
       <c r="G17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -2601,8 +2726,11 @@
       <c r="G18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -2621,8 +2749,11 @@
       <c r="G19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -2636,14 +2767,17 @@
         <v>58</v>
       </c>
       <c r="E20" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G20">
-        <f>D20/2</f>
+        <f t="shared" ref="G20:G43" si="0">D20/2</f>
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -2657,14 +2791,17 @@
         <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G21">
-        <f>D21/2</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -2681,11 +2818,14 @@
         <v>117</v>
       </c>
       <c r="G22">
-        <f>D22/2</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>61</v>
       </c>
@@ -2699,14 +2839,17 @@
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G23">
-        <f>D23/2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -2720,14 +2863,17 @@
         <v>28</v>
       </c>
       <c r="E24" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G24">
-        <f>D24/2</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>65</v>
       </c>
@@ -2741,14 +2887,17 @@
         <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G25">
-        <f>D25/2</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>67</v>
       </c>
@@ -2762,14 +2911,17 @@
         <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G26">
-        <f>D26/2</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>69</v>
       </c>
@@ -2783,14 +2935,17 @@
         <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G27">
-        <f>D27/2</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>71</v>
       </c>
@@ -2804,14 +2959,17 @@
         <v>4</v>
       </c>
       <c r="E28" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G28">
-        <f>D28/2</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>73</v>
       </c>
@@ -2828,11 +2986,14 @@
         <v>118</v>
       </c>
       <c r="G29">
-        <f>D29/2</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>75</v>
       </c>
@@ -2849,11 +3010,14 @@
         <v>117</v>
       </c>
       <c r="G30">
-        <f>D30/2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -2867,14 +3031,17 @@
         <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G31">
-        <f>D31/2</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>79</v>
       </c>
@@ -2888,11 +3055,14 @@
         <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G32">
-        <f>D32/2</f>
+        <f t="shared" si="0"/>
         <v>1</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -2912,8 +3082,11 @@
         <v>117</v>
       </c>
       <c r="G33">
-        <f>D33/2</f>
+        <f t="shared" si="0"/>
         <v>2</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2930,11 +3103,14 @@
         <v>8</v>
       </c>
       <c r="E34" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G34">
-        <f>D34/2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2954,8 +3130,11 @@
         <v>117</v>
       </c>
       <c r="G35">
-        <f>D35/2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2975,7 +3154,7 @@
         <v>117</v>
       </c>
       <c r="G36">
-        <f>D36/2</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H36" t="s">
@@ -2999,7 +3178,7 @@
         <v>117</v>
       </c>
       <c r="G37">
-        <f>D37/2</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H37" t="s">
@@ -3026,7 +3205,7 @@
         <v>10</v>
       </c>
       <c r="G38">
-        <f>D38/2</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H38" t="s">
@@ -3053,7 +3232,7 @@
         <v>10</v>
       </c>
       <c r="G39">
-        <f>D39/2</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H39" t="s">
@@ -3077,7 +3256,7 @@
         <v>117</v>
       </c>
       <c r="G40">
-        <f>D40/2</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H40" t="s">
@@ -3104,7 +3283,7 @@
         <v>10</v>
       </c>
       <c r="G41">
-        <f>D41/2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H41" t="s">
@@ -3131,7 +3310,7 @@
         <v>15</v>
       </c>
       <c r="G42">
-        <f>D42/2</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H42" t="s">
@@ -3158,7 +3337,7 @@
         <v>10</v>
       </c>
       <c r="G43">
-        <f>D43/2</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H43" t="s">
@@ -3332,6 +3511,9 @@
       <c r="G50">
         <v>0</v>
       </c>
+      <c r="H50" s="2" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
@@ -3349,26 +3531,97 @@
       <c r="G51">
         <v>0</v>
       </c>
+      <c r="H51" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>130</v>
+      </c>
+      <c r="C52" t="s">
+        <v>56</v>
+      </c>
+      <c r="D52">
+        <v>4</v>
+      </c>
+      <c r="E52" t="s">
+        <v>118</v>
+      </c>
+      <c r="F52">
+        <v>50</v>
+      </c>
+      <c r="G52">
+        <v>2</v>
+      </c>
+      <c r="H52" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>131</v>
+      </c>
+      <c r="C53" t="s">
+        <v>56</v>
+      </c>
+      <c r="D53">
+        <v>4</v>
+      </c>
+      <c r="E53" t="s">
+        <v>118</v>
+      </c>
+      <c r="F53">
+        <v>50</v>
+      </c>
+      <c r="G53">
+        <v>2</v>
+      </c>
+      <c r="H53" t="s">
+        <v>118</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1" xr:uid="{2F8EA1B3-DE99-4B5B-B92A-5EF6DEBF9FE4}"/>
   <conditionalFormatting sqref="E1:F1048576">
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
       <formula>"CHECK"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
       <formula>"BUY"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H45 H47 H49:H1048576">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+  <conditionalFormatting sqref="H47 H49:H51 H54:H1048576 H1:H45">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>"Picked"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+      <formula>"CHECK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+      <formula>"BUY"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H48">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>"CHECK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+      <formula>"BUY"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H53">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"OK"</formula>
     </cfRule>
@@ -3379,7 +3632,7 @@
       <formula>"BUY"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H48">
+  <conditionalFormatting sqref="H52">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"OK"</formula>
     </cfRule>

</xml_diff>